<commit_message>
openpyxl get_sheet_names and get_sheet_by_name were warning about deprecation; change to use new syntax to access this information.
.gitignore some junk that pycharm creates
</commit_message>
<xml_diff>
--- a/pycounter/test/data/JR1_bad.xlsx
+++ b/pycounter/test/data/JR1_bad.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Techuser\Documents\pycounter\pycounter\test\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\speargh\Documents\pycounter\pycounter\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="230">
   <si>
     <t>Journal Report 1 (R4)</t>
   </si>
@@ -568,21 +568,6 @@
   </si>
   <si>
     <t>2168-6211</t>
-  </si>
-  <si>
-    <t>5708</t>
-  </si>
-  <si>
-    <t>3961</t>
-  </si>
-  <si>
-    <t>1747</t>
-  </si>
-  <si>
-    <t>592</t>
-  </si>
-  <si>
-    <t>574</t>
   </si>
   <si>
     <t>502</t>
@@ -1103,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1113,7 +1098,7 @@
     <col min="3" max="10" width="10.7109375" customWidth="1"/>
     <col min="11" max="11" width="7.7109375" customWidth="1"/>
     <col min="12" max="21" width="5.42578125" customWidth="1"/>
-    <col min="22" max="22" width="6.140625" customWidth="1"/>
+    <col min="22" max="22" width="8.85546875" customWidth="1"/>
     <col min="23" max="23" width="213.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1127,7 +1112,7 @@
     </row>
     <row r="2" spans="1:22" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1190,10 +1175,10 @@
         <v>16</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="M8" s="11" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="N8" s="3" t="s">
         <v>17</v>
@@ -1245,7 +1230,7 @@
         <v>29</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>30</v>
@@ -1809,55 +1794,60 @@
       <c r="G18" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="H18" s="5">
+        <f>5708</f>
+        <v>5708</v>
+      </c>
+      <c r="I18" s="5">
+        <f>3961</f>
+        <v>3961</v>
+      </c>
+      <c r="J18" s="5">
+        <f>1747</f>
+        <v>1747</v>
+      </c>
+      <c r="K18" s="5">
+        <f>592</f>
+        <v>592</v>
+      </c>
+      <c r="L18" s="5">
+        <f>574</f>
+        <v>574</v>
+      </c>
+      <c r="M18" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="I18" s="5" t="s">
+      <c r="N18" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="J18" s="5" t="s">
+      <c r="O18" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="P18" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="L18" s="5" t="s">
+      <c r="Q18" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="M18" s="5" t="s">
+      <c r="R18" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="N18" s="5" t="s">
+      <c r="S18" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="O18" s="5" t="s">
+      <c r="T18" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="P18" s="5" t="s">
+      <c r="U18" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="Q18" s="5" t="s">
+      <c r="V18" s="5" t="s">
         <v>192</v>
-      </c>
-      <c r="R18" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="S18" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="T18" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="U18" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="V18" s="5" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="19" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>42</v>
@@ -1868,60 +1858,60 @@
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="K19" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="L19" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="M19" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="N19" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="J19" s="5" t="s">
+      <c r="O19" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="P19" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="L19" s="5" t="s">
+      <c r="Q19" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="M19" s="5" t="s">
+      <c r="R19" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="N19" s="5" t="s">
+      <c r="S19" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="O19" s="5" t="s">
+      <c r="T19" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="P19" s="5" t="s">
+      <c r="U19" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="Q19" s="5" t="s">
+      <c r="V19" s="5" t="s">
         <v>210</v>
-      </c>
-      <c r="R19" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="S19" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="T19" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="U19" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="V19" s="5" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>42</v>
@@ -1932,52 +1922,52 @@
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="K20" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="L20" s="5" t="s">
         <v>218</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="J20" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="K20" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="L20" s="5" t="s">
-        <v>223</v>
       </c>
       <c r="M20" s="5" t="s">
         <v>86</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="O20" s="5" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="P20" s="5" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="Q20" s="5" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="R20" s="5" t="s">
         <v>160</v>
       </c>
       <c r="S20" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="T20" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="U20" s="5" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="V20" s="5" t="s">
         <v>88</v>

</xml_diff>